<commit_message>
kleine wijzigingen DTP tabel
</commit_message>
<xml_diff>
--- a/src/main/resources/dmn/rangnummerDTP.xlsx
+++ b/src/main/resources/dmn/rangnummerDTP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\han\git\rivm\rvp-business\src\main\resources\dmn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E6CB81CD-6692-4EED-8B4E-2D907E1B4658}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83D2F248-BF12-4B85-AB33-26D33745F1ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29970" yWindow="1170" windowWidth="28800" windowHeight="14340" tabRatio="834" xr2:uid="{4203C9A5-FA6C-4E14-8325-EE7186AD0D41}"/>
+    <workbookView xWindow="29970" yWindow="1170" windowWidth="28800" windowHeight="14340" tabRatio="834" activeTab="2" xr2:uid="{4203C9A5-FA6C-4E14-8325-EE7186AD0D41}"/>
   </bookViews>
   <sheets>
     <sheet name="D" sheetId="21" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1044" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1044" uniqueCount="67">
   <si>
     <t>null</t>
   </si>
@@ -54,27 +54,18 @@
     <t>Leeftijd in dagen</t>
   </si>
   <si>
-    <t>vaccinatie.vaccinSoort</t>
-  </si>
-  <si>
     <t>&gt;= 365</t>
   </si>
   <si>
     <t>rangnummer</t>
   </si>
   <si>
-    <t>hoogste rang</t>
-  </si>
-  <si>
     <t>interval</t>
   </si>
   <si>
     <t>toelichting</t>
   </si>
   <si>
-    <t>vaccinatie.uitvoerdatum</t>
-  </si>
-  <si>
     <t>&gt;= 150</t>
   </si>
   <si>
@@ -87,9 +78,6 @@
     <t>(0 .. 14)</t>
   </si>
   <si>
-    <t>DKTP 3-5-11</t>
-  </si>
-  <si>
     <t>&gt;= 119</t>
   </si>
   <si>
@@ -241,6 +229,21 @@
   </si>
   <si>
     <t>"Gerevaccineerd"</t>
+  </si>
+  <si>
+    <t>component</t>
+  </si>
+  <si>
+    <t>uitvoerdatum</t>
+  </si>
+  <si>
+    <t>DKTP_3_5_11</t>
+  </si>
+  <si>
+    <t>leeftijd in dagen</t>
+  </si>
+  <si>
+    <t>hoogste rangnummer</t>
   </si>
 </sst>
 </file>
@@ -729,9 +732,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38A50B46-6929-4F7E-B14E-DD7ADF5FB023}">
   <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J35" sqref="J35"/>
+      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -747,39 +750,39 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>63</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>65</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>8</v>
-      </c>
       <c r="J1" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>1</v>
@@ -788,7 +791,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>1</v>
@@ -803,13 +806,13 @@
         <v>0</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J2" s="7"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>1</v>
@@ -821,7 +824,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>1</v>
@@ -833,13 +836,13 @@
         <v>0</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="J3" s="7"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>1</v>
@@ -851,7 +854,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>1</v>
@@ -863,13 +866,13 @@
         <v>0</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="J4" s="7"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>1</v>
@@ -878,7 +881,7 @@
         <v>1</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E5" s="3">
         <v>4</v>
@@ -893,13 +896,13 @@
         <v>0</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="J5" s="7"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>1</v>
@@ -923,13 +926,13 @@
         <v>0</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="J6" s="7"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>1</v>
@@ -938,7 +941,7 @@
         <v>0</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>1</v>
@@ -953,13 +956,13 @@
         <v>0</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="J7" s="7"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>1</v>
@@ -968,7 +971,7 @@
         <v>1</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>1</v>
@@ -983,13 +986,13 @@
         <v>0</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="J8" s="7"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>1</v>
@@ -998,7 +1001,7 @@
         <v>0</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>0</v>
@@ -1013,13 +1016,13 @@
         <v>1</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J9" s="7"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>1</v>
@@ -1028,7 +1031,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>0</v>
@@ -1043,13 +1046,13 @@
         <v>1</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J10" s="7"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>1</v>
@@ -1058,7 +1061,7 @@
         <v>0</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E11" s="3">
         <v>1</v>
@@ -1067,143 +1070,143 @@
         <v>1</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="J11" s="7"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C12" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E12" s="3">
         <v>1</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H12" s="4">
         <v>2</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J12" s="7"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C13" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E13" s="3">
         <v>1</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H13" s="4">
         <v>3</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C14" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E14" s="3">
         <v>1</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H14" s="4">
         <v>2</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J14" s="7"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C15" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E15" s="3">
         <v>1</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H15" s="4">
         <v>3</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>1</v>
@@ -1212,7 +1215,7 @@
         <v>1</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E16" s="3">
         <v>1</v>
@@ -1221,19 +1224,19 @@
         <v>1</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="H16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="J16" s="7"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>1</v>
@@ -1242,7 +1245,7 @@
         <v>1</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E17" s="3">
         <v>1</v>
@@ -1251,21 +1254,21 @@
         <v>1</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="H17" s="4">
         <v>3</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>1</v>
@@ -1274,7 +1277,7 @@
         <v>0</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E18" s="3">
         <v>2</v>
@@ -1283,19 +1286,19 @@
         <v>1</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="J18" s="7"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>1</v>
@@ -1304,7 +1307,7 @@
         <v>0</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E19" s="3">
         <v>2</v>
@@ -1313,30 +1316,30 @@
         <v>1</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H19" s="4">
         <v>3</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C20" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E20" s="3">
         <v>3</v>
@@ -1345,28 +1348,28 @@
         <v>1</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="J20" s="7"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C21" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E21" s="3">
         <v>3</v>
@@ -1375,30 +1378,30 @@
         <v>1</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="H21" s="4">
         <v>4</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J21" s="7" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C22" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E22" s="3">
         <v>3</v>
@@ -1407,30 +1410,30 @@
         <v>1</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="H22" s="4">
         <v>6</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J22" s="7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C23" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E23" s="3">
         <v>3</v>
@@ -1439,28 +1442,28 @@
         <v>1</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="H23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="J23" s="7"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C24" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E24" s="3">
         <v>3</v>
@@ -1469,30 +1472,30 @@
         <v>1</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H24" s="4">
         <v>4</v>
       </c>
       <c r="I24" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J24" s="7" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C25" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E25" s="3">
         <v>3</v>
@@ -1501,21 +1504,21 @@
         <v>1</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H25" s="4">
         <v>6</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J25" s="7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>1</v>
@@ -1524,7 +1527,7 @@
         <v>1</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E26" s="3">
         <v>3</v>
@@ -1533,19 +1536,19 @@
         <v>1</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="H26" s="4" t="s">
         <v>0</v>
       </c>
       <c r="I26" s="7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="J26" s="7"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>1</v>
@@ -1554,7 +1557,7 @@
         <v>1</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E27" s="3">
         <v>3</v>
@@ -1563,21 +1566,21 @@
         <v>1</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H27" s="4">
         <v>4</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J27" s="7" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>1</v>
@@ -1586,7 +1589,7 @@
         <v>1</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E28" s="3">
         <v>3</v>
@@ -1595,30 +1598,30 @@
         <v>1</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H28" s="4">
         <v>6</v>
       </c>
       <c r="I28" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J28" s="7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C29" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E29" s="3">
         <v>4</v>
@@ -1633,13 +1636,13 @@
         <v>0</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="J29" s="7"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>1</v>
@@ -1648,7 +1651,7 @@
         <v>1</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E30" s="3">
         <v>4</v>
@@ -1663,22 +1666,22 @@
         <v>0</v>
       </c>
       <c r="I30" s="7" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="J30" s="7"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C31" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E31" s="3">
         <v>4</v>
@@ -1687,28 +1690,28 @@
         <v>1</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H31" s="4" t="s">
         <v>0</v>
       </c>
       <c r="I31" s="7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="J31" s="7"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C32" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E32" s="3">
         <v>4</v>
@@ -1717,28 +1720,28 @@
         <v>1</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H32" s="4" t="s">
         <v>0</v>
       </c>
       <c r="I32" s="7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="J32" s="7"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C33" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E33" s="3">
         <v>4</v>
@@ -1747,19 +1750,19 @@
         <v>1</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="H33" s="4" t="s">
         <v>0</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="J33" s="7"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>1</v>
@@ -1768,7 +1771,7 @@
         <v>1</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E34" s="3">
         <v>4</v>
@@ -1777,28 +1780,28 @@
         <v>1</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="H34" s="4" t="s">
         <v>0</v>
       </c>
       <c r="I34" s="7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="J34" s="7"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B35" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B35" s="3" t="s">
-        <v>46</v>
-      </c>
       <c r="C35" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E35" s="3">
         <v>4</v>
@@ -1807,30 +1810,30 @@
         <v>1</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="H35" s="4">
         <v>5</v>
       </c>
       <c r="I35" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="J35" s="7" t="s">
         <v>61</v>
-      </c>
-      <c r="J35" s="7" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C36" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E36" s="3">
         <v>4</v>
@@ -1839,30 +1842,30 @@
         <v>1</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="H36" s="4">
         <v>5</v>
       </c>
       <c r="I36" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="J36" s="7" t="s">
         <v>61</v>
-      </c>
-      <c r="J36" s="7" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C37" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E37" s="3">
         <v>4</v>
@@ -1871,21 +1874,21 @@
         <v>1</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H37" s="4">
         <v>5</v>
       </c>
       <c r="I37" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="J37" s="7" t="s">
         <v>61</v>
-      </c>
-      <c r="J37" s="7" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>1</v>
@@ -1894,7 +1897,7 @@
         <v>1</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E38" s="3">
         <v>4</v>
@@ -1903,30 +1906,30 @@
         <v>1</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H38" s="4">
         <v>5</v>
       </c>
       <c r="I38" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="J38" s="7" t="s">
         <v>61</v>
-      </c>
-      <c r="J38" s="7" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C39" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E39" s="3">
         <v>4</v>
@@ -1935,30 +1938,30 @@
         <v>1</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="H39" s="4">
         <v>6</v>
       </c>
       <c r="I39" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J39" s="7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C40" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E40" s="3">
         <v>4</v>
@@ -1967,21 +1970,21 @@
         <v>1</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H40" s="4">
         <v>6</v>
       </c>
       <c r="I40" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J40" s="7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>1</v>
@@ -1990,7 +1993,7 @@
         <v>1</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E41" s="3">
         <v>4</v>
@@ -1999,21 +2002,21 @@
         <v>1</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H41" s="4">
         <v>6</v>
       </c>
       <c r="I41" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J41" s="7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>1</v>
@@ -2022,7 +2025,7 @@
         <v>1</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E42" s="3">
         <v>5</v>
@@ -2037,22 +2040,22 @@
         <v>0</v>
       </c>
       <c r="I42" s="7" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="J42" s="7"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C43" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E43" s="3">
         <v>5</v>
@@ -2061,28 +2064,28 @@
         <v>1</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H43" s="4" t="s">
         <v>0</v>
       </c>
       <c r="I43" s="7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="J43" s="7"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C44" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E44" s="3">
         <v>5</v>
@@ -2091,19 +2094,19 @@
         <v>1</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="H44" s="4" t="s">
         <v>0</v>
       </c>
       <c r="I44" s="7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="J44" s="7"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>1</v>
@@ -2112,7 +2115,7 @@
         <v>1</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E45" s="3">
         <v>5</v>
@@ -2121,28 +2124,28 @@
         <v>1</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="H45" s="4" t="s">
         <v>0</v>
       </c>
       <c r="I45" s="7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="J45" s="7"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C46" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E46" s="3">
         <v>5</v>
@@ -2151,30 +2154,30 @@
         <v>1</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="H46" s="4">
         <v>6</v>
       </c>
       <c r="I46" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J46" s="7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C47" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E47" s="3">
         <v>5</v>
@@ -2183,21 +2186,21 @@
         <v>1</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H47" s="4">
         <v>6</v>
       </c>
       <c r="I47" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J47" s="7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>1</v>
@@ -2206,7 +2209,7 @@
         <v>1</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E48" s="3">
         <v>5</v>
@@ -2215,16 +2218,16 @@
         <v>1</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H48" s="4">
         <v>6</v>
       </c>
       <c r="I48" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J48" s="7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
@@ -2259,8 +2262,8 @@
   <dimension ref="A1:J49"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J42" sqref="J42:J45"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2276,39 +2279,39 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>63</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>65</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>8</v>
-      </c>
       <c r="J1" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>1</v>
@@ -2317,7 +2320,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>1</v>
@@ -2332,13 +2335,13 @@
         <v>0</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J2" s="7"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>1</v>
@@ -2350,7 +2353,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>1</v>
@@ -2362,13 +2365,13 @@
         <v>0</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="J3" s="7"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>1</v>
@@ -2380,7 +2383,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>1</v>
@@ -2392,13 +2395,13 @@
         <v>0</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="J4" s="7"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>1</v>
@@ -2407,7 +2410,7 @@
         <v>1</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E5" s="3">
         <v>4</v>
@@ -2422,13 +2425,13 @@
         <v>0</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="J5" s="7"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>1</v>
@@ -2452,13 +2455,13 @@
         <v>0</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="J6" s="7"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>1</v>
@@ -2467,7 +2470,7 @@
         <v>0</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>1</v>
@@ -2482,13 +2485,13 @@
         <v>0</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="J7" s="7"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>1</v>
@@ -2497,7 +2500,7 @@
         <v>1</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>1</v>
@@ -2512,13 +2515,13 @@
         <v>0</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="J8" s="7"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>1</v>
@@ -2527,7 +2530,7 @@
         <v>0</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>0</v>
@@ -2542,13 +2545,13 @@
         <v>1</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J9" s="7"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>1</v>
@@ -2557,7 +2560,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>0</v>
@@ -2572,13 +2575,13 @@
         <v>1</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J10" s="7"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>1</v>
@@ -2587,7 +2590,7 @@
         <v>0</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E11" s="3">
         <v>1</v>
@@ -2596,143 +2599,143 @@
         <v>1</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="J11" s="7"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C12" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E12" s="3">
         <v>1</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H12" s="4">
         <v>2</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J12" s="7"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C13" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E13" s="3">
         <v>1</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H13" s="4">
         <v>3</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C14" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E14" s="3">
         <v>1</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H14" s="4">
         <v>2</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J14" s="7"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C15" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E15" s="3">
         <v>1</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H15" s="4">
         <v>3</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>1</v>
@@ -2741,7 +2744,7 @@
         <v>1</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E16" s="3">
         <v>1</v>
@@ -2750,19 +2753,19 @@
         <v>1</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="H16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="J16" s="7"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>1</v>
@@ -2771,7 +2774,7 @@
         <v>1</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E17" s="3">
         <v>1</v>
@@ -2780,21 +2783,21 @@
         <v>1</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="H17" s="4">
         <v>3</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>1</v>
@@ -2803,7 +2806,7 @@
         <v>0</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E18" s="3">
         <v>2</v>
@@ -2812,19 +2815,19 @@
         <v>1</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="J18" s="7"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>1</v>
@@ -2833,7 +2836,7 @@
         <v>0</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E19" s="3">
         <v>2</v>
@@ -2842,30 +2845,30 @@
         <v>1</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H19" s="4">
         <v>3</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C20" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E20" s="3">
         <v>3</v>
@@ -2874,28 +2877,28 @@
         <v>1</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="J20" s="7"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C21" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E21" s="3">
         <v>3</v>
@@ -2904,30 +2907,30 @@
         <v>1</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="H21" s="4">
         <v>4</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J21" s="7" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C22" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E22" s="3">
         <v>3</v>
@@ -2936,30 +2939,30 @@
         <v>1</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="H22" s="4">
         <v>6</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J22" s="7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C23" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E23" s="3">
         <v>3</v>
@@ -2968,28 +2971,28 @@
         <v>1</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="H23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="J23" s="7"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C24" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E24" s="3">
         <v>3</v>
@@ -2998,30 +3001,30 @@
         <v>1</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H24" s="4">
         <v>4</v>
       </c>
       <c r="I24" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J24" s="7" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C25" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E25" s="3">
         <v>3</v>
@@ -3030,21 +3033,21 @@
         <v>1</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H25" s="4">
         <v>6</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J25" s="7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>1</v>
@@ -3053,7 +3056,7 @@
         <v>1</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E26" s="3">
         <v>3</v>
@@ -3062,19 +3065,19 @@
         <v>1</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="H26" s="4" t="s">
         <v>0</v>
       </c>
       <c r="I26" s="7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="J26" s="7"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>1</v>
@@ -3083,7 +3086,7 @@
         <v>1</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E27" s="3">
         <v>3</v>
@@ -3092,21 +3095,21 @@
         <v>1</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H27" s="4">
         <v>4</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J27" s="7" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>1</v>
@@ -3115,7 +3118,7 @@
         <v>1</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E28" s="3">
         <v>3</v>
@@ -3124,30 +3127,30 @@
         <v>1</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H28" s="4">
         <v>6</v>
       </c>
       <c r="I28" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J28" s="7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C29" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E29" s="3">
         <v>4</v>
@@ -3162,13 +3165,13 @@
         <v>0</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="J29" s="7"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>1</v>
@@ -3177,7 +3180,7 @@
         <v>1</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E30" s="3">
         <v>4</v>
@@ -3192,22 +3195,22 @@
         <v>0</v>
       </c>
       <c r="I30" s="7" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="J30" s="7"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C31" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E31" s="3">
         <v>4</v>
@@ -3216,28 +3219,28 @@
         <v>1</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H31" s="4" t="s">
         <v>0</v>
       </c>
       <c r="I31" s="7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="J31" s="7"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C32" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E32" s="3">
         <v>4</v>
@@ -3246,28 +3249,28 @@
         <v>1</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H32" s="4" t="s">
         <v>0</v>
       </c>
       <c r="I32" s="7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="J32" s="7"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C33" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E33" s="3">
         <v>4</v>
@@ -3276,19 +3279,19 @@
         <v>1</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="H33" s="4" t="s">
         <v>0</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="J33" s="7"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>1</v>
@@ -3297,7 +3300,7 @@
         <v>1</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E34" s="3">
         <v>4</v>
@@ -3306,28 +3309,28 @@
         <v>1</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="H34" s="4" t="s">
         <v>0</v>
       </c>
       <c r="I34" s="7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="J34" s="7"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C35" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E35" s="3">
         <v>4</v>
@@ -3336,30 +3339,30 @@
         <v>1</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="H35" s="4">
         <v>5</v>
       </c>
       <c r="I35" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="J35" s="7" t="s">
         <v>61</v>
-      </c>
-      <c r="J35" s="7" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C36" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E36" s="3">
         <v>4</v>
@@ -3368,30 +3371,30 @@
         <v>1</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="H36" s="4">
         <v>5</v>
       </c>
       <c r="I36" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="J36" s="7" t="s">
         <v>61</v>
-      </c>
-      <c r="J36" s="7" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C37" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E37" s="3">
         <v>4</v>
@@ -3400,21 +3403,21 @@
         <v>1</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H37" s="4">
         <v>5</v>
       </c>
       <c r="I37" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="J37" s="7" t="s">
         <v>61</v>
-      </c>
-      <c r="J37" s="7" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>1</v>
@@ -3423,7 +3426,7 @@
         <v>1</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E38" s="3">
         <v>4</v>
@@ -3432,30 +3435,30 @@
         <v>1</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H38" s="4">
         <v>5</v>
       </c>
       <c r="I38" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="J38" s="7" t="s">
         <v>61</v>
-      </c>
-      <c r="J38" s="7" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C39" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E39" s="3">
         <v>4</v>
@@ -3464,30 +3467,30 @@
         <v>1</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="H39" s="4">
         <v>6</v>
       </c>
       <c r="I39" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J39" s="7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C40" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E40" s="3">
         <v>4</v>
@@ -3496,21 +3499,21 @@
         <v>1</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H40" s="4">
         <v>6</v>
       </c>
       <c r="I40" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J40" s="7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>1</v>
@@ -3519,7 +3522,7 @@
         <v>1</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E41" s="3">
         <v>4</v>
@@ -3528,21 +3531,21 @@
         <v>1</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H41" s="4">
         <v>6</v>
       </c>
       <c r="I41" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J41" s="7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>1</v>
@@ -3551,7 +3554,7 @@
         <v>1</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E42" s="3">
         <v>5</v>
@@ -3566,22 +3569,22 @@
         <v>0</v>
       </c>
       <c r="I42" s="7" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="J42" s="7"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C43" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E43" s="3">
         <v>5</v>
@@ -3590,28 +3593,28 @@
         <v>1</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H43" s="4" t="s">
         <v>0</v>
       </c>
       <c r="I43" s="7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="J43" s="7"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C44" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E44" s="3">
         <v>5</v>
@@ -3620,19 +3623,19 @@
         <v>1</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="H44" s="4" t="s">
         <v>0</v>
       </c>
       <c r="I44" s="7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="J44" s="7"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>1</v>
@@ -3641,7 +3644,7 @@
         <v>1</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E45" s="3">
         <v>5</v>
@@ -3650,28 +3653,28 @@
         <v>1</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="H45" s="4" t="s">
         <v>0</v>
       </c>
       <c r="I45" s="7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="J45" s="7"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C46" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E46" s="3">
         <v>5</v>
@@ -3680,30 +3683,30 @@
         <v>1</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="H46" s="4">
         <v>6</v>
       </c>
       <c r="I46" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J46" s="7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C47" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E47" s="3">
         <v>5</v>
@@ -3712,21 +3715,21 @@
         <v>1</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H47" s="4">
         <v>6</v>
       </c>
       <c r="I47" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J47" s="7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>1</v>
@@ -3735,7 +3738,7 @@
         <v>1</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E48" s="3">
         <v>5</v>
@@ -3744,16 +3747,16 @@
         <v>1</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H48" s="4">
         <v>6</v>
       </c>
       <c r="I48" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J48" s="7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
@@ -3787,9 +3790,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B592DA3-47C3-4820-9B5C-427EAA5D9F83}">
   <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I46" sqref="I46:I48"/>
+      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3805,39 +3808,39 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>63</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>8</v>
-      </c>
       <c r="J1" s="6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>1</v>
@@ -3846,7 +3849,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>1</v>
@@ -3861,13 +3864,13 @@
         <v>0</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J2" s="7"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>1</v>
@@ -3879,7 +3882,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>1</v>
@@ -3891,13 +3894,13 @@
         <v>0</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="J3" s="7"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>1</v>
@@ -3909,7 +3912,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>1</v>
@@ -3921,13 +3924,13 @@
         <v>0</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="J4" s="7"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>1</v>
@@ -3936,7 +3939,7 @@
         <v>1</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E5" s="3">
         <v>4</v>
@@ -3951,13 +3954,13 @@
         <v>0</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="J5" s="7"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>1</v>
@@ -3981,13 +3984,13 @@
         <v>0</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="J6" s="7"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>1</v>
@@ -3996,7 +3999,7 @@
         <v>0</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>1</v>
@@ -4011,13 +4014,13 @@
         <v>0</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="J7" s="7"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>1</v>
@@ -4026,7 +4029,7 @@
         <v>1</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>1</v>
@@ -4041,13 +4044,13 @@
         <v>0</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="J8" s="7"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>1</v>
@@ -4056,7 +4059,7 @@
         <v>0</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>0</v>
@@ -4071,13 +4074,13 @@
         <v>1</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J9" s="7"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>1</v>
@@ -4086,7 +4089,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>0</v>
@@ -4101,13 +4104,13 @@
         <v>1</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J10" s="7"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>1</v>
@@ -4116,7 +4119,7 @@
         <v>0</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E11" s="3">
         <v>1</v>
@@ -4125,143 +4128,143 @@
         <v>1</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H11" s="4" t="s">
         <v>0</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="J11" s="7"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C12" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E12" s="3">
         <v>1</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H12" s="4">
         <v>2</v>
       </c>
       <c r="I12" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J12" s="7"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C13" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E13" s="3">
         <v>1</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H13" s="4">
         <v>3</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C14" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E14" s="3">
         <v>1</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H14" s="4">
         <v>2</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J14" s="7"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C15" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E15" s="3">
         <v>1</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H15" s="4">
         <v>3</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J15" s="7" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>1</v>
@@ -4270,7 +4273,7 @@
         <v>1</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E16" s="3">
         <v>1</v>
@@ -4279,19 +4282,19 @@
         <v>1</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="H16" s="4" t="s">
         <v>0</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="J16" s="7"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>1</v>
@@ -4300,7 +4303,7 @@
         <v>1</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E17" s="3">
         <v>1</v>
@@ -4309,21 +4312,21 @@
         <v>1</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="H17" s="4">
         <v>3</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>1</v>
@@ -4332,7 +4335,7 @@
         <v>0</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E18" s="3">
         <v>2</v>
@@ -4341,19 +4344,19 @@
         <v>1</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="J18" s="7"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>1</v>
@@ -4362,7 +4365,7 @@
         <v>0</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E19" s="3">
         <v>2</v>
@@ -4371,30 +4374,30 @@
         <v>1</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H19" s="4">
         <v>3</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C20" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E20" s="3">
         <v>3</v>
@@ -4403,28 +4406,28 @@
         <v>1</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H20" s="4" t="s">
         <v>0</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="J20" s="7"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C21" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E21" s="3">
         <v>3</v>
@@ -4433,30 +4436,30 @@
         <v>1</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="H21" s="4">
         <v>4</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J21" s="7" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C22" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E22" s="3">
         <v>3</v>
@@ -4465,30 +4468,30 @@
         <v>1</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="H22" s="4">
         <v>6</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J22" s="7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C23" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E23" s="3">
         <v>3</v>
@@ -4497,28 +4500,28 @@
         <v>1</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="H23" s="4" t="s">
         <v>0</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="J23" s="7"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C24" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E24" s="3">
         <v>3</v>
@@ -4527,30 +4530,30 @@
         <v>1</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H24" s="4">
         <v>4</v>
       </c>
       <c r="I24" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J24" s="7" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C25" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E25" s="3">
         <v>3</v>
@@ -4559,21 +4562,21 @@
         <v>1</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H25" s="4">
         <v>6</v>
       </c>
       <c r="I25" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J25" s="7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>1</v>
@@ -4582,7 +4585,7 @@
         <v>1</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E26" s="3">
         <v>3</v>
@@ -4591,19 +4594,19 @@
         <v>1</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="H26" s="4" t="s">
         <v>0</v>
       </c>
       <c r="I26" s="7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="J26" s="7"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>1</v>
@@ -4612,7 +4615,7 @@
         <v>1</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E27" s="3">
         <v>3</v>
@@ -4621,21 +4624,21 @@
         <v>1</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H27" s="4">
         <v>4</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J27" s="7" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>1</v>
@@ -4644,7 +4647,7 @@
         <v>1</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E28" s="3">
         <v>3</v>
@@ -4653,30 +4656,30 @@
         <v>1</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H28" s="4">
         <v>6</v>
       </c>
       <c r="I28" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J28" s="7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C29" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E29" s="3">
         <v>4</v>
@@ -4691,13 +4694,13 @@
         <v>0</v>
       </c>
       <c r="I29" s="7" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="J29" s="7"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>1</v>
@@ -4706,7 +4709,7 @@
         <v>1</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E30" s="3">
         <v>4</v>
@@ -4721,22 +4724,22 @@
         <v>0</v>
       </c>
       <c r="I30" s="7" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="J30" s="7"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C31" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E31" s="3">
         <v>4</v>
@@ -4745,28 +4748,28 @@
         <v>1</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H31" s="4" t="s">
         <v>0</v>
       </c>
       <c r="I31" s="7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="J31" s="7"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C32" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E32" s="3">
         <v>4</v>
@@ -4775,28 +4778,28 @@
         <v>1</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H32" s="4" t="s">
         <v>0</v>
       </c>
       <c r="I32" s="7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="J32" s="7"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C33" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E33" s="3">
         <v>4</v>
@@ -4805,19 +4808,19 @@
         <v>1</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="H33" s="4" t="s">
         <v>0</v>
       </c>
       <c r="I33" s="7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="J33" s="7"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>1</v>
@@ -4826,7 +4829,7 @@
         <v>1</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E34" s="3">
         <v>4</v>
@@ -4835,28 +4838,28 @@
         <v>1</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="H34" s="4" t="s">
         <v>0</v>
       </c>
       <c r="I34" s="7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="J34" s="7"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C35" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E35" s="3">
         <v>4</v>
@@ -4865,30 +4868,30 @@
         <v>1</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="H35" s="4">
         <v>5</v>
       </c>
       <c r="I35" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="J35" s="7" t="s">
         <v>61</v>
-      </c>
-      <c r="J35" s="7" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C36" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E36" s="3">
         <v>4</v>
@@ -4897,30 +4900,30 @@
         <v>1</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="H36" s="4">
         <v>5</v>
       </c>
       <c r="I36" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="J36" s="7" t="s">
         <v>61</v>
-      </c>
-      <c r="J36" s="7" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C37" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E37" s="3">
         <v>4</v>
@@ -4929,21 +4932,21 @@
         <v>1</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H37" s="4">
         <v>5</v>
       </c>
       <c r="I37" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="J37" s="7" t="s">
         <v>61</v>
-      </c>
-      <c r="J37" s="7" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>1</v>
@@ -4952,7 +4955,7 @@
         <v>1</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E38" s="3">
         <v>4</v>
@@ -4961,30 +4964,30 @@
         <v>1</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H38" s="4">
         <v>5</v>
       </c>
       <c r="I38" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="J38" s="7" t="s">
         <v>61</v>
-      </c>
-      <c r="J38" s="7" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C39" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E39" s="3">
         <v>4</v>
@@ -4993,30 +4996,30 @@
         <v>1</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="H39" s="4">
         <v>6</v>
       </c>
       <c r="I39" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J39" s="7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C40" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E40" s="3">
         <v>4</v>
@@ -5025,21 +5028,21 @@
         <v>1</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H40" s="4">
         <v>6</v>
       </c>
       <c r="I40" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J40" s="7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>1</v>
@@ -5048,7 +5051,7 @@
         <v>1</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E41" s="3">
         <v>4</v>
@@ -5057,21 +5060,21 @@
         <v>1</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H41" s="4">
         <v>6</v>
       </c>
       <c r="I41" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J41" s="7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>1</v>
@@ -5080,7 +5083,7 @@
         <v>1</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E42" s="3">
         <v>5</v>
@@ -5095,22 +5098,22 @@
         <v>0</v>
       </c>
       <c r="I42" s="7" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="J42" s="7"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C43" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E43" s="3">
         <v>5</v>
@@ -5119,28 +5122,28 @@
         <v>1</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H43" s="4" t="s">
         <v>0</v>
       </c>
       <c r="I43" s="7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="J43" s="7"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C44" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E44" s="3">
         <v>5</v>
@@ -5149,19 +5152,19 @@
         <v>1</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="H44" s="4" t="s">
         <v>0</v>
       </c>
       <c r="I44" s="7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="J44" s="7"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>1</v>
@@ -5170,7 +5173,7 @@
         <v>1</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E45" s="3">
         <v>5</v>
@@ -5179,28 +5182,28 @@
         <v>1</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="H45" s="4" t="s">
         <v>0</v>
       </c>
       <c r="I45" s="7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="J45" s="7"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C46" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E46" s="3">
         <v>5</v>
@@ -5209,30 +5212,30 @@
         <v>1</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="H46" s="4">
         <v>6</v>
       </c>
       <c r="I46" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J46" s="7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C47" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E47" s="3">
         <v>5</v>
@@ -5241,21 +5244,21 @@
         <v>1</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H47" s="4">
         <v>6</v>
       </c>
       <c r="I47" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J47" s="7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>1</v>
@@ -5264,7 +5267,7 @@
         <v>1</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E48" s="3">
         <v>5</v>
@@ -5273,16 +5276,16 @@
         <v>1</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H48" s="4">
         <v>6</v>
       </c>
       <c r="I48" s="7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J48" s="7" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>